<commit_message>
data visualization is totally ready for the cars which are not fired
</commit_message>
<xml_diff>
--- a/ceza_almayan_araclar.xlsx
+++ b/ceza_almayan_araclar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>52.20153254455276</v>
+        <v>33.54101966249685</v>
       </c>
     </row>
     <row r="3">
@@ -451,15 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>42.72001872658765</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>61.84658438426491</v>
+        <v>31.6227766016838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some problems are solved.Ready for testing
</commit_message>
<xml_diff>
--- a/ceza_almayan_araclar.xlsx
+++ b/ceza_almayan_araclar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,14 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>33.54101966249685</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>31.6227766016838</v>
       </c>
     </row>

</xml_diff>

<commit_message>
the property of deleting the file automatically is imported
</commit_message>
<xml_diff>
--- a/ceza_almayan_araclar.xlsx
+++ b/ceza_almayan_araclar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,6 @@
         <v>33.54101966249685</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>31.6227766016838</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
The adjustments are being applied to the physical system
</commit_message>
<xml_diff>
--- a/ceza_almayan_araclar.xlsx
+++ b/ceza_almayan_araclar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,119 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>42.72001872658765</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>45.27692569068709</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>35.35533905932738</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>46.09772228646444</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>47.43416490252569</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>36.40054944640259</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
         <v>31.6227766016838</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>44.7213595499958</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>43.01162633521314</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>47.16990566028302</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>41.23105625617661</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>32.01562118716424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the property of taking screenshot has been improved
</commit_message>
<xml_diff>
--- a/ceza_almayan_araclar.xlsx
+++ b/ceza_almayan_araclar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>42.72001872658765</v>
+        <v>45.27692569068709</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>45.27692569068709</v>
+        <v>53.15072906367325</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>35.35533905932738</v>
+        <v>43.01162633521314</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>40</v>
+        <v>50.99019513592785</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>35</v>
+        <v>25.49509756796392</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>46.09772228646444</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>47.43416490252569</v>
+        <v>46.09772228646444</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>36.40054944640259</v>
+        <v>49.49747468305833</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>31.6227766016838</v>
+        <v>39.05124837953327</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>44.7213595499958</v>
+        <v>40.31128874149275</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>43.01162633521314</v>
+        <v>47.43416490252569</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>47.16990566028302</v>
+        <v>30.4138126514911</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>30</v>
+        <v>36.40054944640259</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>41.23105625617661</v>
+        <v>55.90169943749475</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,63 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>32.01562118716424</v>
+        <v>52.20153254455276</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>49.24428900898052</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>55.22680508593631</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>31.6227766016838</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>54.08326913195985</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>38.07886552931955</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>53.85164807134504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The function for the graphs representing cars that have not been fired has been improved
</commit_message>
<xml_diff>
--- a/ceza_almayan_araclar.xlsx
+++ b/ceza_almayan_araclar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>45.27692569068709</v>
+        <v>42.42640687119285</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>53.15072906367325</v>
+        <v>43.01162633521314</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>43.01162633521314</v>
+        <v>33.54101966249685</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>50.99019513592785</v>
+        <v>40.31128874149275</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>25.49509756796392</v>
+        <v>31.6227766016838</v>
       </c>
     </row>
     <row r="7">
@@ -483,135 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>46.09772228646444</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>49.49747468305833</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>39.05124837953327</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>40.31128874149275</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>47.43416490252569</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>30.4138126514911</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>36.40054944640259</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>55.90169943749475</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>52.20153254455276</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>49.24428900898052</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>55.22680508593631</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>31.6227766016838</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>54.08326913195985</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>38.07886552931955</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>53.85164807134504</v>
+        <v>44.7213595499958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>